<commit_message>
Template selection to be changed from Binary to XML
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestMethods_New/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestMethods_New/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\KTOC-TRB-Automation\KTOC_TRB_TestMethods\src\com\KTOC\TRB\testautomation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\KTOC-TRB-Automation\KTOC_TRB_TestMethods_New\src\com\KTOC\TRB\testautomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D400268A-B8D7-4004-8721-42B61F3881AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9290B6EB-49F0-4D29-B630-3D031420714C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -208,9 +208,6 @@
     <t>Sherbrooke</t>
   </si>
   <si>
-    <t>AutomationSFA</t>
-  </si>
-  <si>
     <t>AUTOMATION TRB CKQ</t>
   </si>
   <si>
@@ -257,6 +254,9 @@
   </si>
   <si>
     <t>AutomationKTOC SFA</t>
+  </si>
+  <si>
+    <t>AutomationSFA_XML</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -760,13 +762,13 @@
         <v>48</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>29</v>
@@ -783,7 +785,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="4">
         <v>1723</v>
@@ -819,7 +821,7 @@
         <v>51</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>47</v>
@@ -828,13 +830,13 @@
         <v>49</v>
       </c>
       <c r="Q2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>33</v>
@@ -883,7 +885,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -961,13 +965,13 @@
         <v>48</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>29</v>
@@ -984,7 +988,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4">
         <v>1813</v>
@@ -1029,13 +1033,13 @@
         <v>49</v>
       </c>
       <c r="Q2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>33</v>
@@ -1084,7 +1088,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1173,13 +1179,13 @@
         <v>48</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>29</v>
@@ -1196,7 +1202,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4">
         <v>1723</v>
@@ -1241,7 +1247,7 @@
         <v>51</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>47</v>
@@ -1250,13 +1256,13 @@
         <v>49</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>33</v>

</xml_diff>